<commit_message>
50 persen attendance update
</commit_message>
<xml_diff>
--- a/public/images/UKM Odd/Balawarta Gimmik.xlsx
+++ b/public/images/UKM Odd/Balawarta Gimmik.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3999" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4002" uniqueCount="347">
   <si>
     <t>NIM</t>
   </si>
@@ -5871,7 +5871,23 @@
         <v>11.0</v>
       </c>
     </row>
-    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1">
+      <c r="A54" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="E54" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
     <row r="55" ht="14.25" customHeight="1"/>
     <row r="56" ht="14.25" customHeight="1"/>
     <row r="57" ht="14.25" customHeight="1"/>

</xml_diff>